<commit_message>
Alterado dicionario de dados
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionario_dados final.xlsx
+++ b/dicionario_dados/dicionario_dados final.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="saldoestoque" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="110">
   <si>
     <t>Tabela</t>
   </si>
@@ -63,27 +63,9 @@
     <t>X</t>
   </si>
   <si>
-    <t>Clustered</t>
-  </si>
-  <si>
-    <t>NonClustered</t>
-  </si>
-  <si>
-    <t>Unique</t>
-  </si>
-  <si>
-    <t>Colunas</t>
-  </si>
-  <si>
     <t>Valor min e max</t>
   </si>
   <si>
-    <t>Índice</t>
-  </si>
-  <si>
-    <t>Nome do índice</t>
-  </si>
-  <si>
     <t>saldoestoque</t>
   </si>
   <si>
@@ -111,9 +93,6 @@
     <t>Coluna com a quantidade de peças no estoque</t>
   </si>
   <si>
-    <t>idx_id_saldo_estoque</t>
-  </si>
-  <si>
     <t>item</t>
   </si>
   <si>
@@ -175,9 +154,6 @@
   </si>
   <si>
     <t>Código identificador do status do item</t>
-  </si>
-  <si>
-    <t>idx_id_item</t>
   </si>
   <si>
     <t>0 - 2.147.483.647</t>
@@ -514,6 +490,12 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -531,12 +513,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -844,7 +820,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -852,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,52 +845,52 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
@@ -930,15 +906,15 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="18"/>
       <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
@@ -946,19 +922,19 @@
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="A6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="18"/>
       <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -966,19 +942,19 @@
         <v>10</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="20"/>
+      <c r="A7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="22"/>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>9</v>
@@ -986,62 +962,11 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="F9:H9"/>
+  <mergeCells count="7">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
@@ -1049,7 +974,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:H8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1072,10 +996,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,52 +1014,52 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>5</v>
@@ -1151,15 +1075,15 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="18"/>
       <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
@@ -1167,19 +1091,19 @@
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="D6" s="12" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>9</v>
@@ -1187,19 +1111,19 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="20"/>
+      <c r="A7" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="22"/>
       <c r="C7" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>9</v>
@@ -1207,19 +1131,19 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="20"/>
+      <c r="A8" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="22"/>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>9</v>
@@ -1227,141 +1151,87 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="20"/>
+      <c r="A9" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="22"/>
       <c r="C9" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="20"/>
+      <c r="A10" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="22"/>
       <c r="C10" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="20"/>
+      <c r="A11" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="22"/>
       <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="20"/>
+      <c r="A12" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="22"/>
       <c r="C12" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="F14:H14"/>
+  <mergeCells count="12">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
@@ -1371,7 +1241,9 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1380,10 +1252,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,52 +1267,52 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>5</v>
@@ -1456,15 +1328,15 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="18"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
@@ -1472,16 +1344,16 @@
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="A6" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="18"/>
       <c r="C6" s="8" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D6" s="12">
         <v>50</v>
@@ -1492,65 +1364,17 @@
         <v>10</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A6:B6"/>
+  <mergeCells count="6">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1558,10 +1382,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,52 +1398,52 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>5</v>
@@ -1635,200 +1459,152 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="18"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="8"/>
-      <c r="H5" s="21" t="s">
-        <v>57</v>
+      <c r="H5" s="15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="A6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="18"/>
       <c r="C6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="21" t="s">
-        <v>63</v>
+      <c r="H6" s="15" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="16"/>
+      <c r="A7" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="18"/>
       <c r="C7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="21" t="s">
-        <v>64</v>
+      <c r="H7" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="8" t="s">
-        <v>59</v>
-      </c>
       <c r="D8" s="12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="21" t="s">
-        <v>65</v>
+      <c r="H8" s="15" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="16"/>
+      <c r="A9" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="18"/>
       <c r="C9" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="21" t="s">
-        <v>66</v>
+      <c r="H9" s="15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="16"/>
+      <c r="A10" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="18"/>
       <c r="C10" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="16"/>
+      <c r="H10" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="18"/>
       <c r="C11" s="8" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="H11" s="15" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A11:B11"/>
+  <mergeCells count="11">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A9:B9"/>
   </mergeCells>
@@ -1838,10 +1614,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,52 +1630,52 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>5</v>
@@ -1915,15 +1691,15 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="18"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>9</v>
@@ -1933,19 +1709,19 @@
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="A6" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="18"/>
       <c r="C6" s="8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>9</v>
@@ -1954,66 +1730,18 @@
       <c r="G6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="H6" s="15" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A6:B6"/>
+  <mergeCells count="6">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2021,10 +1749,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2037,52 +1765,52 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>5</v>
@@ -2098,15 +1826,15 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="18"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>9</v>
@@ -2115,20 +1843,20 @@
         <v>10</v>
       </c>
       <c r="G5" s="8"/>
-      <c r="H5" s="21" t="s">
-        <v>75</v>
+      <c r="H5" s="15" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="A6" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="18"/>
       <c r="C6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>9</v>
@@ -2137,125 +1865,77 @@
       <c r="G6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="21" t="s">
-        <v>76</v>
+      <c r="H6" s="15" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7" s="16"/>
+      <c r="A7" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="18"/>
       <c r="C7" s="8" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="21" t="s">
-        <v>78</v>
+      <c r="H7" s="15" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="16"/>
+      <c r="A8" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="18"/>
       <c r="C8" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="21" t="s">
-        <v>82</v>
+      <c r="H8" s="15" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="16"/>
+      <c r="A9" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="18"/>
       <c r="C9" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="H9" s="15" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:H10"/>
+  <mergeCells count="9">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2263,10 +1943,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2279,52 +1959,52 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>5</v>
@@ -2340,15 +2020,15 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="18"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>9</v>
@@ -2357,107 +2037,59 @@
         <v>10</v>
       </c>
       <c r="G5" s="8"/>
-      <c r="H5" s="21" t="s">
-        <v>87</v>
+      <c r="H5" s="15" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="A6" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="18"/>
       <c r="C6" s="8" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="21" t="s">
-        <v>88</v>
+      <c r="H6" s="15" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="16"/>
+      <c r="A7" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="18"/>
       <c r="C7" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="H7" s="15" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A7:B7"/>
+  <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2465,10 +2097,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2481,52 +2113,52 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>5</v>
@@ -2542,15 +2174,15 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="18"/>
       <c r="C5" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>9</v>
@@ -2560,85 +2192,37 @@
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="11" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="A6" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="18"/>
       <c r="C6" s="8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="H6" s="16" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A6:B6"/>
+  <mergeCells count="6">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2646,10 +2230,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2662,52 +2246,52 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>5</v>
@@ -2723,15 +2307,15 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="16"/>
+      <c r="A5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="18"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>9</v>
@@ -2740,86 +2324,38 @@
         <v>10</v>
       </c>
       <c r="G5" s="8"/>
-      <c r="H5" s="21" t="s">
-        <v>98</v>
+      <c r="H5" s="15" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="16"/>
+      <c r="A6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="18"/>
       <c r="C6" s="8" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="21" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="H6" s="15" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A6:B6"/>
+  <mergeCells count="6">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>